<commit_message>
Se agregó verificación elemento existente en el carrito de compra
</commit_message>
<xml_diff>
--- a/data/Esquema BD SuperAndes.xlsx
+++ b/data/Esquema BD SuperAndes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juanestebanmendez/Documents/Los Andes/Sistrans/b-09/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\Documentos\2018-2\Sistemas Transaccionales\Proyecto\Iteración 2\superandes\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C79E020-5885-8945-90DA-F0577EDF9D05}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9613D718-6924-4E3D-BBB5-8F148A349DDC}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16460" xr2:uid="{982294D2-D2C2-3040-83F6-7FBF7CDC620E}"/>
+    <workbookView xWindow="0" yWindow="456" windowWidth="28800" windowHeight="16464" xr2:uid="{982294D2-D2C2-3040-83F6-7FBF7CDC620E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="92">
   <si>
     <t>id</t>
   </si>
@@ -292,13 +292,35 @@
   </si>
   <si>
     <t>CK(&gt;0)</t>
+  </si>
+  <si>
+    <t>CARRITOCOMPRAS</t>
+  </si>
+  <si>
+    <t>estado</t>
+  </si>
+  <si>
+    <t>VENDECARRITO</t>
+  </si>
+  <si>
+    <t>idCarrito</t>
+  </si>
+  <si>
+    <t>PK
+FK (Carritocompras.id)</t>
+  </si>
+  <si>
+    <t>FK (Vende.id)</t>
+  </si>
+  <si>
+    <t>cantidadCarrito</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -983,31 +1005,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{256ABFA4-8E9A-C240-8C23-4C6EDDC69B8B}">
-  <dimension ref="A1:O44"/>
+  <dimension ref="A1:O56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E55" sqref="E55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.5" customWidth="1"/>
-    <col min="2" max="2" width="13.83203125" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="18.83203125" customWidth="1"/>
+    <col min="2" max="2" width="13.796875" customWidth="1"/>
+    <col min="3" max="3" width="15.69921875" customWidth="1"/>
+    <col min="4" max="4" width="18.796875" customWidth="1"/>
     <col min="5" max="5" width="19.5" customWidth="1"/>
-    <col min="6" max="6" width="17.33203125" customWidth="1"/>
-    <col min="7" max="7" width="21.6640625" customWidth="1"/>
+    <col min="6" max="6" width="17.296875" customWidth="1"/>
+    <col min="7" max="7" width="21.69921875" customWidth="1"/>
     <col min="8" max="8" width="24.5" customWidth="1"/>
-    <col min="9" max="9" width="22.1640625" customWidth="1"/>
-    <col min="10" max="10" width="20.6640625" customWidth="1"/>
+    <col min="9" max="9" width="22.19921875" customWidth="1"/>
+    <col min="10" max="10" width="20.69921875" customWidth="1"/>
     <col min="11" max="11" width="14" customWidth="1"/>
-    <col min="12" max="12" width="19.33203125" customWidth="1"/>
-    <col min="13" max="13" width="24.6640625" customWidth="1"/>
-    <col min="14" max="14" width="13.1640625" customWidth="1"/>
+    <col min="12" max="12" width="19.296875" customWidth="1"/>
+    <col min="13" max="13" width="24.69921875" customWidth="1"/>
+    <col min="14" max="14" width="13.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="17" thickBot="1">
+    <row r="1" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
@@ -1027,7 +1049,7 @@
       <c r="N1" s="12"/>
       <c r="O1" s="12"/>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
@@ -1072,7 +1094,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
@@ -1117,7 +1139,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="35" customHeight="1" thickBot="1">
+    <row r="4" spans="1:15" ht="34.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
         <v>48</v>
       </c>
@@ -1160,7 +1182,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="12"/>
       <c r="B5" s="12"/>
       <c r="C5" s="12"/>
@@ -1175,7 +1197,7 @@
       <c r="L5" s="12"/>
       <c r="O5" s="12"/>
     </row>
-    <row r="6" spans="1:15" ht="17" thickBot="1">
+    <row r="6" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="15" t="s">
         <v>8</v>
       </c>
@@ -1195,7 +1217,7 @@
       <c r="N6" s="12"/>
       <c r="O6" s="12"/>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
         <v>0</v>
       </c>
@@ -1226,7 +1248,7 @@
       <c r="N7" s="12"/>
       <c r="O7" s="12"/>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>1</v>
       </c>
@@ -1257,7 +1279,7 @@
       <c r="N8" s="12"/>
       <c r="O8" s="12"/>
     </row>
-    <row r="9" spans="1:15" ht="35" thickBot="1">
+    <row r="9" spans="1:15" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="6" t="s">
         <v>48</v>
       </c>
@@ -1289,7 +1311,7 @@
       <c r="N9" s="12"/>
       <c r="O9" s="12"/>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="12"/>
       <c r="B10" s="12"/>
       <c r="C10" s="12"/>
@@ -1304,7 +1326,7 @@
       <c r="N10" s="12"/>
       <c r="O10" s="12"/>
     </row>
-    <row r="11" spans="1:15" ht="17" thickBot="1">
+    <row r="11" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="12" t="s">
         <v>9</v>
       </c>
@@ -1324,7 +1346,7 @@
       <c r="N11" s="12"/>
       <c r="O11" s="12"/>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
         <v>0</v>
       </c>
@@ -1362,7 +1384,7 @@
       </c>
       <c r="O12" s="12"/>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>1</v>
       </c>
@@ -1400,7 +1422,7 @@
       </c>
       <c r="O13" s="12"/>
     </row>
-    <row r="14" spans="1:15" ht="35" thickBot="1">
+    <row r="14" spans="1:15" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="6" t="s">
         <v>48</v>
       </c>
@@ -1434,7 +1456,7 @@
       <c r="N14" s="8"/>
       <c r="O14" s="12"/>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" s="12"/>
       <c r="B15" s="12"/>
       <c r="C15" s="12"/>
@@ -1444,7 +1466,7 @@
       <c r="G15" s="12"/>
       <c r="O15" s="12"/>
     </row>
-    <row r="16" spans="1:15" ht="17" thickBot="1">
+    <row r="16" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>10</v>
       </c>
@@ -1462,7 +1484,7 @@
       <c r="M16" s="1"/>
       <c r="O16" s="12"/>
     </row>
-    <row r="17" spans="1:15">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" s="9" t="s">
         <v>0</v>
       </c>
@@ -1497,7 +1519,7 @@
       <c r="N17" s="12"/>
       <c r="O17" s="12"/>
     </row>
-    <row r="18" spans="1:15">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>1</v>
       </c>
@@ -1532,7 +1554,7 @@
       <c r="N18" s="12"/>
       <c r="O18" s="12"/>
     </row>
-    <row r="19" spans="1:15" ht="17" thickBot="1">
+    <row r="19" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="6" t="s">
         <v>48</v>
       </c>
@@ -1567,7 +1589,7 @@
       <c r="N19" s="12"/>
       <c r="O19" s="12"/>
     </row>
-    <row r="20" spans="1:15">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="F20" s="12"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
@@ -1578,7 +1600,7 @@
       <c r="M20" s="12"/>
       <c r="O20" s="12"/>
     </row>
-    <row r="21" spans="1:15" ht="17" thickBot="1">
+    <row r="21" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>61</v>
       </c>
@@ -1592,7 +1614,7 @@
       <c r="L21" s="12"/>
       <c r="O21" s="12"/>
     </row>
-    <row r="22" spans="1:15">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" s="9" t="s">
         <v>3</v>
       </c>
@@ -1629,7 +1651,7 @@
       </c>
       <c r="O22" s="12"/>
     </row>
-    <row r="23" spans="1:15">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>1</v>
       </c>
@@ -1666,7 +1688,7 @@
       </c>
       <c r="O23" s="12"/>
     </row>
-    <row r="24" spans="1:15" ht="32" customHeight="1" thickBot="1">
+    <row r="24" spans="1:15" ht="31.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="20" t="s">
         <v>62</v>
       </c>
@@ -1703,10 +1725,10 @@
       </c>
       <c r="O24" s="12"/>
     </row>
-    <row r="25" spans="1:15">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="O25" s="12"/>
     </row>
-    <row r="26" spans="1:15" ht="17" thickBot="1">
+    <row r="26" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="14" t="s">
         <v>11</v>
       </c>
@@ -1723,7 +1745,7 @@
       <c r="J26" s="16"/>
       <c r="O26" s="12"/>
     </row>
-    <row r="27" spans="1:15">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27" s="9" t="s">
         <v>0</v>
       </c>
@@ -1755,7 +1777,7 @@
       <c r="L27" s="12"/>
       <c r="O27" s="12"/>
     </row>
-    <row r="28" spans="1:15">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
         <v>1</v>
       </c>
@@ -1787,7 +1809,7 @@
       <c r="L28" s="12"/>
       <c r="O28" s="12"/>
     </row>
-    <row r="29" spans="1:15" ht="33" customHeight="1" thickBot="1">
+    <row r="29" spans="1:15" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="17" t="s">
         <v>48</v>
       </c>
@@ -1819,7 +1841,7 @@
       <c r="L29" s="12"/>
       <c r="O29" s="12"/>
     </row>
-    <row r="30" spans="1:15">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A30" s="12"/>
       <c r="B30" s="12"/>
       <c r="E30" s="12"/>
@@ -1827,7 +1849,7 @@
       <c r="G30" s="12"/>
       <c r="O30" s="12"/>
     </row>
-    <row r="31" spans="1:15" ht="17" thickBot="1">
+    <row r="31" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="14" t="s">
         <v>12</v>
       </c>
@@ -1838,7 +1860,7 @@
       <c r="G31" s="12"/>
       <c r="O31" s="12"/>
     </row>
-    <row r="32" spans="1:15">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32" s="9" t="s">
         <v>0</v>
       </c>
@@ -1858,7 +1880,7 @@
       <c r="N32" s="12"/>
       <c r="O32" s="12"/>
     </row>
-    <row r="33" spans="1:15">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
         <v>1</v>
       </c>
@@ -1878,7 +1900,7 @@
       <c r="N33" s="12"/>
       <c r="O33" s="12"/>
     </row>
-    <row r="34" spans="1:15" ht="32" customHeight="1" thickBot="1">
+    <row r="34" spans="1:15" ht="31.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="17" t="s">
         <v>48</v>
       </c>
@@ -1898,12 +1920,12 @@
       <c r="N34" s="12"/>
       <c r="O34" s="12"/>
     </row>
-    <row r="35" spans="1:15">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A35" s="12"/>
       <c r="B35" s="12"/>
       <c r="G35" s="28"/>
     </row>
-    <row r="36" spans="1:15" ht="17" thickBot="1">
+    <row r="36" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>63</v>
       </c>
@@ -1912,7 +1934,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="37" spans="1:15">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A37" s="9" t="s">
         <v>16</v>
       </c>
@@ -1933,7 +1955,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="38" spans="1:15">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
         <v>1</v>
       </c>
@@ -1954,7 +1976,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:15" ht="35" thickBot="1">
+    <row r="39" spans="1:15" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="20" t="s">
         <v>55</v>
       </c>
@@ -1975,7 +1997,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="41" spans="1:15" ht="17" thickBot="1">
+    <row r="41" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="3" t="s">
         <v>76</v>
       </c>
@@ -1983,7 +2005,7 @@
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
     </row>
-    <row r="42" spans="1:15">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A42" s="9" t="s">
         <v>0</v>
       </c>
@@ -2000,7 +2022,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="1:15">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A43" s="4" t="s">
         <v>1</v>
       </c>
@@ -2017,7 +2039,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:15" ht="52" thickBot="1">
+    <row r="44" spans="1:15" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="20" t="s">
         <v>48</v>
       </c>
@@ -2034,6 +2056,87 @@
       <c r="G44" s="27" t="s">
         <v>79</v>
       </c>
+    </row>
+    <row r="47" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A48" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B48" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="C48" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D48" s="10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="B50" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="C50" s="21"/>
+      <c r="D50" s="21" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="B54" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C54" s="10" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A56" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="B56" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="C56" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Se agrego requerimiento 'Devolver producto' en el carrito de compras y se actualizo archivo excel con Esquema de la BD
</commit_message>
<xml_diff>
--- a/data/Esquema BD SuperAndes.xlsx
+++ b/data/Esquema BD SuperAndes.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juanestebanmendez/Documents/Los Andes/Sistrans/b-09/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juanestebanmendez/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C79E020-5885-8945-90DA-F0577EDF9D05}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F13080BA-BC29-B347-A9C5-F288F82D836B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16460" xr2:uid="{982294D2-D2C2-3040-83F6-7FBF7CDC620E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="91">
   <si>
     <t>id</t>
   </si>
@@ -272,11 +272,6 @@
     <t>fechaFin</t>
   </si>
   <si>
-    <t>VER SI AÑADIR TIPO
-Crear tabla en BD
-Uniadades</t>
-  </si>
-  <si>
     <t>CATEGORIASUCURSAL</t>
   </si>
   <si>
@@ -292,6 +287,28 @@
   </si>
   <si>
     <t>CK(&gt;0)</t>
+  </si>
+  <si>
+    <t>CARRITOCOMPRAS</t>
+  </si>
+  <si>
+    <t>estado</t>
+  </si>
+  <si>
+    <t>VENDECARRITO</t>
+  </si>
+  <si>
+    <t>idCarrito</t>
+  </si>
+  <si>
+    <t>PK
+FK (Carritocompras.id)</t>
+  </si>
+  <si>
+    <t>FK (Vende.id)</t>
+  </si>
+  <si>
+    <t>cantidadCarrito</t>
   </si>
 </sst>
 </file>
@@ -560,7 +577,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -637,9 +654,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -983,13 +997,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{256ABFA4-8E9A-C240-8C23-4C6EDDC69B8B}">
-  <dimension ref="A1:O44"/>
+  <dimension ref="A1:O56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="17.5" customWidth="1"/>
     <col min="2" max="2" width="13.83203125" customWidth="1"/>
@@ -1141,13 +1155,13 @@
         <v>50</v>
       </c>
       <c r="I4" s="25" t="s">
+        <v>82</v>
+      </c>
+      <c r="J4" s="25" t="s">
         <v>83</v>
       </c>
-      <c r="J4" s="25" t="s">
-        <v>84</v>
-      </c>
       <c r="K4" s="25" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="L4" s="21" t="s">
         <v>72</v>
@@ -1183,7 +1197,7 @@
       <c r="C6" s="13"/>
       <c r="D6" s="12"/>
       <c r="F6" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I6" s="14" t="s">
         <v>14</v>
@@ -1199,14 +1213,12 @@
       <c r="A7" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="11" t="s">
-        <v>3</v>
-      </c>
+      <c r="C7" s="12"/>
       <c r="D7" s="12"/>
-      <c r="F7" s="30" t="s">
+      <c r="F7" s="29" t="s">
         <v>4</v>
       </c>
       <c r="G7" s="11" t="s">
@@ -1230,12 +1242,10 @@
       <c r="A8" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>1</v>
-      </c>
+      <c r="C8" s="12"/>
       <c r="D8" s="12"/>
       <c r="F8" s="4" t="s">
         <v>1</v>
@@ -1261,19 +1271,17 @@
       <c r="A9" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="C9" s="8" t="s">
-        <v>50</v>
-      </c>
+      <c r="C9" s="12"/>
       <c r="D9" s="12"/>
       <c r="E9" s="16"/>
-      <c r="F9" s="32" t="s">
+      <c r="F9" s="31" t="s">
+        <v>80</v>
+      </c>
+      <c r="G9" s="30" t="s">
         <v>81</v>
-      </c>
-      <c r="G9" s="31" t="s">
-        <v>82</v>
       </c>
       <c r="I9" s="6" t="s">
         <v>48</v>
@@ -1320,7 +1328,7 @@
       </c>
       <c r="K11" s="12"/>
       <c r="L11" s="12"/>
-      <c r="M11" s="29"/>
+      <c r="M11" s="28"/>
       <c r="N11" s="12"/>
       <c r="O11" s="12"/>
     </row>
@@ -1551,16 +1559,16 @@
       <c r="F19" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="G19" s="36" t="s">
+      <c r="G19" s="35" t="s">
         <v>58</v>
       </c>
-      <c r="H19" s="36" t="s">
+      <c r="H19" s="35" t="s">
         <v>73</v>
       </c>
-      <c r="I19" s="36" t="s">
+      <c r="I19" s="35" t="s">
         <v>73</v>
       </c>
-      <c r="J19" s="37" t="s">
+      <c r="J19" s="36" t="s">
         <v>49</v>
       </c>
       <c r="M19" s="12"/>
@@ -1608,7 +1616,7 @@
       <c r="E22" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="F22" s="33" t="s">
+      <c r="F22" s="32" t="s">
         <v>32</v>
       </c>
       <c r="G22" s="16"/>
@@ -1645,7 +1653,7 @@
       <c r="E23" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F23" s="34" t="s">
+      <c r="F23" s="33" t="s">
         <v>1</v>
       </c>
       <c r="G23" s="16"/>
@@ -1682,7 +1690,7 @@
       <c r="E24" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="F24" s="35" t="s">
+      <c r="F24" s="34" t="s">
         <v>74</v>
       </c>
       <c r="G24" s="16"/>
@@ -1901,7 +1909,7 @@
     <row r="35" spans="1:15">
       <c r="A35" s="12"/>
       <c r="B35" s="12"/>
-      <c r="G35" s="28"/>
+      <c r="G35" s="27"/>
     </row>
     <row r="36" spans="1:15" ht="17" thickBot="1">
       <c r="A36" t="s">
@@ -2031,9 +2039,87 @@
       <c r="E44" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="G44" s="27" t="s">
-        <v>79</v>
-      </c>
+    </row>
+    <row r="47" spans="1:15" ht="17" thickBot="1">
+      <c r="A47" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15">
+      <c r="A48" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B48" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="C48" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D48" s="10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="18" thickBot="1">
+      <c r="A50" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="B50" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="C50" s="21"/>
+      <c r="D50" s="21" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="17" thickBot="1">
+      <c r="A53" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="B54" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C54" s="10" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="52" thickBot="1">
+      <c r="A56" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="B56" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="C56" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Se agrego soporte para añadir promoción en la interfaz
</commit_message>
<xml_diff>
--- a/data/Esquema BD SuperAndes.xlsx
+++ b/data/Esquema BD SuperAndes.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juanestebanmendez/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juanestebanmendez/Documents/Los Andes/Sistrans/superandes/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F13080BA-BC29-B347-A9C5-F288F82D836B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29E7E47C-2F9D-D148-9565-66E9AE0A73D8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16460" xr2:uid="{982294D2-D2C2-3040-83F6-7FBF7CDC620E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="94">
   <si>
     <t>id</t>
   </si>
@@ -309,6 +309,15 @@
   </si>
   <si>
     <t>cantidadCarrito</t>
+  </si>
+  <si>
+    <t>cantidadProductosVendidos</t>
+  </si>
+  <si>
+    <t>cantidadProductos</t>
+  </si>
+  <si>
+    <t>FK(Proveedor.id)</t>
   </si>
 </sst>
 </file>
@@ -365,7 +374,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -573,11 +582,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -682,6 +702,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -999,8 +1028,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{256ABFA4-8E9A-C240-8C23-4C6EDDC69B8B}">
   <dimension ref="A1:O56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="G44" sqref="G44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16"/>
@@ -2002,26 +2031,42 @@
         <v>77</v>
       </c>
       <c r="D42" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="E42" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="E42" s="11" t="s">
+      <c r="F42" s="10" t="s">
         <v>3</v>
+      </c>
+      <c r="G42" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="H42" s="11" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="43" spans="1:15">
       <c r="A43" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B43" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="B43" s="2"/>
       <c r="C43" s="2" t="s">
         <v>36</v>
       </c>
       <c r="D43" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E43" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E43" s="5" t="s">
+      <c r="F43" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G43" s="38" t="s">
+        <v>1</v>
+      </c>
+      <c r="H43" s="5" t="s">
         <v>1</v>
       </c>
     </row>
@@ -2036,9 +2081,14 @@
         <v>49</v>
       </c>
       <c r="D44" s="21"/>
-      <c r="E44" s="19" t="s">
+      <c r="E44" s="21"/>
+      <c r="F44" s="18" t="s">
         <v>50</v>
       </c>
+      <c r="G44" s="39" t="s">
+        <v>93</v>
+      </c>
+      <c r="H44" s="21"/>
     </row>
     <row r="47" spans="1:15" ht="17" thickBot="1">
       <c r="A47" t="s">

</xml_diff>